<commit_message>
Création du projet principal et de l'interface
</commit_message>
<xml_diff>
--- a/Livrables/David Dubey Journal de travail Pré TPI.xlsx
+++ b/Livrables/David Dubey Journal de travail Pré TPI.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr showObjects="none" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David.DUBEY\Documents\GitHub\Pre-TPI-2021-Labyrinthe\Livrables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David.DUBEY\Documents\GitHub\Pre-TPI-Labyrinthe-Unity\Livrables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
   <si>
     <t>Début</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>Changement de moteur, installation de Unity</t>
+  </si>
+  <si>
+    <t>Changement de Github</t>
+  </si>
+  <si>
+    <t>Création</t>
+  </si>
+  <si>
+    <t>Création d'un projet de test</t>
+  </si>
+  <si>
+    <t>Création du projet principal et création de l'interface</t>
   </si>
 </sst>
 </file>
@@ -1026,8 +1038,8 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,37 +1461,72 @@
       <c r="B18" s="4">
         <v>0.38611111111111113</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="D18" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>44258.000463078701</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="G18" s="3"/>
+        <v>0.1243055555555555</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+      <c r="A19" s="5">
+        <v>44259</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="D19" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="G19" s="3"/>
+        <v>4.9305555555555491E-2</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="5">
+        <v>44260</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.62430555555555556</v>
+      </c>
       <c r="D20" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="G20" s="3"/>
+        <v>0.17986111111111114</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1800,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1876,6 +1923,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update David Dubey Journal de travail Pré TPI.xlsx
</commit_message>
<xml_diff>
--- a/Livrables/David Dubey Journal de travail Pré TPI.xlsx
+++ b/Livrables/David Dubey Journal de travail Pré TPI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
   <si>
     <t>Début</t>
   </si>
@@ -131,6 +131,15 @@
   </si>
   <si>
     <t>Création du projet principal et création de l'interface</t>
+  </si>
+  <si>
+    <t>Remise à jour du nouveau Github</t>
+  </si>
+  <si>
+    <t>Rédaction documentation</t>
+  </si>
+  <si>
+    <t>Avancement sur le jeu</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1047,8 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,27 +1539,47 @@
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+      <c r="A21" s="5">
+        <v>44265</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.41805555555555557</v>
+      </c>
       <c r="D21" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="G21" s="3"/>
+        <v>8.1944444444444486E-2</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="5">
+        <v>44265</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.44097222222222227</v>
+      </c>
       <c r="D22" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="G22" s="3"/>
+        <v>2.2916666666666696E-2</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1847,10 +1876,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,6 +1960,14 @@
         <v>34</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Avancement documentation de projet
</commit_message>
<xml_diff>
--- a/Livrables/David Dubey Journal de travail Pré TPI.xlsx
+++ b/Livrables/David Dubey Journal de travail Pré TPI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
   <si>
     <t>Début</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Avancement sur le jeu</t>
+  </si>
+  <si>
+    <t>Avancement sur la documentation</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1051,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,15 +1586,25 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="5">
+        <v>44266</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.62638888888888888</v>
+      </c>
       <c r="D23" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="G23" s="3"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Création graphique de la nouvelle planification
</commit_message>
<xml_diff>
--- a/Livrables/David Dubey Journal de travail Pré TPI.xlsx
+++ b/Livrables/David Dubey Journal de travail Pré TPI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>Début</t>
   </si>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,15 +1608,25 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="A24" s="5">
+        <v>44267</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.62708333333333333</v>
+      </c>
       <c r="D24" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="G24" s="3"/>
+        <v>6.0416666666666674E-2</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Avancement sur le jeu
</commit_message>
<xml_diff>
--- a/Livrables/David Dubey Journal de travail Pré TPI.xlsx
+++ b/Livrables/David Dubey Journal de travail Pré TPI.xlsx
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,19 +1661,23 @@
       <c r="C26" s="4"/>
       <c r="D26" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>44272.000598032406</v>
+        <v>44274.067861342592</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="5">
+        <v>44274</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.44236111111111115</v>
+      </c>
       <c r="C27" s="4"/>
       <c r="D27" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
+        <v>44274.000500231479</v>
       </c>
       <c r="E27" s="6"/>
       <c r="G27" s="3"/>

</xml_diff>

<commit_message>
avancement sur la doc
</commit_message>
<xml_diff>
--- a/Livrables/David Dubey Journal de travail Pré TPI.xlsx
+++ b/Livrables/David Dubey Journal de travail Pré TPI.xlsx
@@ -1050,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,7 +1661,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>44274.067861342592</v>
+        <v>44277.071851157409</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="3"/>
@@ -1677,14 +1677,16 @@
       <c r="C27" s="4"/>
       <c r="D27" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>44274.000500231479</v>
+        <v>44277.004490046296</v>
       </c>
       <c r="E27" s="6"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+      <c r="A28" s="5">
+        <v>44277</v>
+      </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="11">

</xml_diff>

<commit_message>
Ajout du system de drag and drop
</commit_message>
<xml_diff>
--- a/Livrables/David Dubey Journal de travail Pré TPI.xlsx
+++ b/Livrables/David Dubey Journal de travail Pré TPI.xlsx
@@ -1050,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,7 +1661,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>44277.071851157409</v>
+        <v>44279.009171296297</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="3"/>
@@ -1677,7 +1677,7 @@
       <c r="C27" s="4"/>
       <c r="D27" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>44277.004490046296</v>
+        <v>44278.941810185184</v>
       </c>
       <c r="E27" s="6"/>
       <c r="G27" s="3"/>
@@ -1698,12 +1698,16 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="5">
+        <v>44279</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.36805555555555558</v>
+      </c>
       <c r="C29" s="4"/>
       <c r="D29" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
+        <v>44279.016115740742</v>
       </c>
       <c r="E29" s="6"/>
       <c r="G29" s="3"/>

</xml_diff>

<commit_message>
Avancement sur la documentation
</commit_message>
<xml_diff>
--- a/Livrables/David Dubey Journal de travail Pré TPI.xlsx
+++ b/Livrables/David Dubey Journal de travail Pré TPI.xlsx
@@ -1661,7 +1661,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>44279.009171296297</v>
+        <v>44281.074114120369</v>
       </c>
       <c r="E26" s="6"/>
       <c r="G26" s="3"/>
@@ -1677,7 +1677,7 @@
       <c r="C27" s="4"/>
       <c r="D27" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>44278.941810185184</v>
+        <v>44281.006753009256</v>
       </c>
       <c r="E27" s="6"/>
       <c r="G27" s="3"/>
@@ -1707,19 +1707,23 @@
       <c r="C29" s="4"/>
       <c r="D29" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>44279.016115740742</v>
+        <v>44281.081058564814</v>
       </c>
       <c r="E29" s="6"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="5">
+        <v>44281</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.44861111111111113</v>
+      </c>
       <c r="C30" s="4"/>
       <c r="D30" s="11">
         <f ca="1">IF(ISBLANK(Tableau1[[#This Row],[Fin]]), NOW(),Tableau1[[#This Row],[Fin]])-IF(ISBLANK(Tableau1[[#This Row],[Début]]),NOW(),Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
+        <v>44281.000503009258</v>
       </c>
       <c r="E30" s="6"/>
       <c r="G30" s="3"/>

</xml_diff>